<commit_message>
incluye resource pool y shifts
</commit_message>
<xml_diff>
--- a/InputCMPC.xlsx
+++ b/InputCMPC.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24426"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ite02\Documents\Gaston\CMPC-manufacturing\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EC552BB-66AF-4E0E-A37C-DB15C27A0080}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16695" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16700" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -247,10 +241,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="mmm"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="mmm"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -258,6 +252,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -640,18 +635,18 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="284" applyFont="1"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="284" applyFont="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="284" applyFont="1"/>
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" xfId="284" applyFont="1"/>
   </cellXfs>
   <cellStyles count="285">
     <cellStyle name="60% - Accent1" xfId="1" builtinId="32"/>
@@ -1274,14 +1269,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S40"/>
   <sheetViews>
     <sheetView topLeftCell="A5" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection sqref="A1:S40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="21" style="2" customWidth="1"/>
     <col min="2" max="13" width="0" hidden="1" customWidth="1"/>
@@ -1289,7 +1284,7 @@
     <col min="19" max="19" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" s="4" customFormat="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1348,7 +1343,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1407,7 +1402,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -1466,7 +1461,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -1525,7 +1520,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -1584,7 +1579,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -1643,7 +1638,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -1702,7 +1697,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -1761,7 +1756,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -1820,7 +1815,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
@@ -1879,7 +1874,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
@@ -1938,7 +1933,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
@@ -1997,7 +1992,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
@@ -2056,7 +2051,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
@@ -2115,7 +2110,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
@@ -2174,7 +2169,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
@@ -2233,7 +2228,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19">
       <c r="A17" s="2" t="s">
         <v>16</v>
       </c>
@@ -2292,7 +2287,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19">
       <c r="A18" s="2" t="s">
         <v>17</v>
       </c>
@@ -2351,7 +2346,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19">
       <c r="A19" s="2" t="s">
         <v>18</v>
       </c>
@@ -2410,7 +2405,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19">
       <c r="A20" s="2" t="s">
         <v>19</v>
       </c>
@@ -2469,7 +2464,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19">
       <c r="A21" s="2" t="s">
         <v>20</v>
       </c>
@@ -2528,7 +2523,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19">
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
@@ -2587,7 +2582,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19">
       <c r="A23" s="2" t="s">
         <v>22</v>
       </c>
@@ -2646,7 +2641,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19">
       <c r="A24" s="2" t="s">
         <v>23</v>
       </c>
@@ -2705,7 +2700,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19">
       <c r="A25" s="2" t="s">
         <v>24</v>
       </c>
@@ -2764,7 +2759,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19">
       <c r="A26" s="2" t="s">
         <v>25</v>
       </c>
@@ -2823,7 +2818,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19">
       <c r="A27" s="2" t="s">
         <v>26</v>
       </c>
@@ -2882,7 +2877,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19">
       <c r="A28" s="2" t="s">
         <v>27</v>
       </c>
@@ -2941,7 +2936,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19">
       <c r="A29" s="2" t="s">
         <v>28</v>
       </c>
@@ -3000,7 +2995,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19">
       <c r="A30" s="2" t="s">
         <v>29</v>
       </c>
@@ -3059,7 +3054,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19">
       <c r="A31" s="2" t="s">
         <v>30</v>
       </c>
@@ -3118,7 +3113,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19">
       <c r="A32" s="2" t="s">
         <v>31</v>
       </c>
@@ -3177,7 +3172,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19">
       <c r="A33" s="2" t="s">
         <v>32</v>
       </c>
@@ -3236,7 +3231,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19">
       <c r="A34" s="2" t="s">
         <v>33</v>
       </c>
@@ -3295,7 +3290,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19">
       <c r="A35" s="2" t="s">
         <v>34</v>
       </c>
@@ -3354,7 +3349,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19">
       <c r="A36" s="2" t="s">
         <v>35</v>
       </c>
@@ -3413,7 +3408,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19">
       <c r="A37" s="2" t="s">
         <v>36</v>
       </c>
@@ -3472,7 +3467,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19">
       <c r="A38" s="2" t="s">
         <v>37</v>
       </c>
@@ -3531,7 +3526,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19">
       <c r="A39" s="2" t="s">
         <v>38</v>
       </c>
@@ -3590,7 +3585,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:19">
       <c r="A40" s="2" t="s">
         <v>39</v>
       </c>
@@ -3661,27 +3656,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z469"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J469" sqref="J2:J469"/>
+    <sheetView tabSelected="1" topLeftCell="A183" workbookViewId="0">
+      <selection activeCell="X201" sqref="X201"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="22.5" customWidth="1"/>
-    <col min="2" max="2" width="9.125" customWidth="1"/>
-    <col min="3" max="3" width="20.875" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" customWidth="1"/>
+    <col min="3" max="3" width="20.83203125" customWidth="1"/>
     <col min="4" max="7" width="13" customWidth="1"/>
     <col min="8" max="8" width="16" style="5" customWidth="1"/>
     <col min="9" max="9" width="13" customWidth="1"/>
-    <col min="10" max="10" width="12.375" customWidth="1"/>
+    <col min="10" max="10" width="12.33203125" customWidth="1"/>
     <col min="11" max="22" width="0" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="11.625" customWidth="1"/>
+    <col min="23" max="23" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26">
       <c r="A1" t="s">
         <v>58</v>
       </c>
@@ -3722,7 +3717,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -3770,7 +3765,7 @@
       <c r="Y2" s="4"/>
       <c r="Z2" s="4"/>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -3802,7 +3797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -3834,7 +3829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
@@ -3866,7 +3861,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26">
       <c r="A6" s="2" t="s">
         <v>1</v>
       </c>
@@ -3898,7 +3893,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26">
       <c r="A7" s="2" t="s">
         <v>1</v>
       </c>
@@ -3930,7 +3925,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26">
       <c r="A8" s="2" t="s">
         <v>1</v>
       </c>
@@ -3962,7 +3957,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26">
       <c r="A9" s="2" t="s">
         <v>1</v>
       </c>
@@ -3994,7 +3989,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26">
       <c r="A10" s="2" t="s">
         <v>1</v>
       </c>
@@ -4026,7 +4021,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
@@ -4058,7 +4053,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26">
       <c r="A12" s="2" t="s">
         <v>1</v>
       </c>
@@ -4090,7 +4085,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26">
       <c r="A13" s="2" t="s">
         <v>1</v>
       </c>
@@ -4158,7 +4153,7 @@
         <v>236.32090194917032</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26">
       <c r="A14" s="2" t="s">
         <v>2</v>
       </c>
@@ -4190,7 +4185,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26">
       <c r="A15" s="2" t="s">
         <v>2</v>
       </c>
@@ -4222,7 +4217,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26">
       <c r="A16" s="2" t="s">
         <v>2</v>
       </c>
@@ -4254,7 +4249,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10">
       <c r="A17" s="2" t="s">
         <v>2</v>
       </c>
@@ -4286,7 +4281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10">
       <c r="A18" s="2" t="s">
         <v>2</v>
       </c>
@@ -4318,7 +4313,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10">
       <c r="A19" s="2" t="s">
         <v>2</v>
       </c>
@@ -4350,7 +4345,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10">
       <c r="A20" s="2" t="s">
         <v>2</v>
       </c>
@@ -4382,7 +4377,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10">
       <c r="A21" s="2" t="s">
         <v>2</v>
       </c>
@@ -4414,7 +4409,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10">
       <c r="A22" s="2" t="s">
         <v>2</v>
       </c>
@@ -4446,7 +4441,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10">
       <c r="A23" s="2" t="s">
         <v>2</v>
       </c>
@@ -4478,7 +4473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10">
       <c r="A24" s="2" t="s">
         <v>2</v>
       </c>
@@ -4510,7 +4505,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10">
       <c r="A25" s="2" t="s">
         <v>2</v>
       </c>
@@ -4542,7 +4537,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10">
       <c r="A26" s="2" t="s">
         <v>3</v>
       </c>
@@ -4574,7 +4569,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10">
       <c r="A27" s="2" t="s">
         <v>3</v>
       </c>
@@ -4606,7 +4601,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10">
       <c r="A28" s="2" t="s">
         <v>3</v>
       </c>
@@ -4638,7 +4633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10">
       <c r="A29" s="2" t="s">
         <v>3</v>
       </c>
@@ -4670,7 +4665,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10">
       <c r="A30" s="2" t="s">
         <v>3</v>
       </c>
@@ -4702,7 +4697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10">
       <c r="A31" s="2" t="s">
         <v>3</v>
       </c>
@@ -4734,7 +4729,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10">
       <c r="A32" s="2" t="s">
         <v>3</v>
       </c>
@@ -4766,7 +4761,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10">
       <c r="A33" s="2" t="s">
         <v>3</v>
       </c>
@@ -4798,7 +4793,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10">
       <c r="A34" s="2" t="s">
         <v>3</v>
       </c>
@@ -4830,7 +4825,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10">
       <c r="A35" s="2" t="s">
         <v>3</v>
       </c>
@@ -4862,7 +4857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10">
       <c r="A36" s="2" t="s">
         <v>3</v>
       </c>
@@ -4894,7 +4889,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10">
       <c r="A37" s="2" t="s">
         <v>3</v>
       </c>
@@ -4926,7 +4921,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10">
       <c r="A38" s="2" t="s">
         <v>4</v>
       </c>
@@ -4958,7 +4953,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10">
       <c r="A39" s="2" t="s">
         <v>4</v>
       </c>
@@ -4990,7 +4985,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10">
       <c r="A40" s="2" t="s">
         <v>4</v>
       </c>
@@ -5022,7 +5017,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10">
       <c r="A41" s="2" t="s">
         <v>4</v>
       </c>
@@ -5054,7 +5049,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10">
       <c r="A42" s="2" t="s">
         <v>4</v>
       </c>
@@ -5086,7 +5081,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10">
       <c r="A43" s="2" t="s">
         <v>4</v>
       </c>
@@ -5118,7 +5113,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10">
       <c r="A44" s="2" t="s">
         <v>4</v>
       </c>
@@ -5150,7 +5145,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10">
       <c r="A45" s="2" t="s">
         <v>4</v>
       </c>
@@ -5182,7 +5177,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10">
       <c r="A46" s="2" t="s">
         <v>4</v>
       </c>
@@ -5214,7 +5209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10">
       <c r="A47" s="2" t="s">
         <v>4</v>
       </c>
@@ -5246,7 +5241,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10">
       <c r="A48" s="2" t="s">
         <v>4</v>
       </c>
@@ -5278,7 +5273,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10">
       <c r="A49" s="2" t="s">
         <v>4</v>
       </c>
@@ -5310,7 +5305,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10">
       <c r="A50" s="2" t="s">
         <v>5</v>
       </c>
@@ -5342,7 +5337,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10">
       <c r="A51" s="2" t="s">
         <v>5</v>
       </c>
@@ -5374,7 +5369,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10">
       <c r="A52" s="2" t="s">
         <v>5</v>
       </c>
@@ -5406,7 +5401,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10">
       <c r="A53" s="2" t="s">
         <v>5</v>
       </c>
@@ -5438,7 +5433,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10">
       <c r="A54" s="2" t="s">
         <v>5</v>
       </c>
@@ -5470,7 +5465,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10">
       <c r="A55" s="2" t="s">
         <v>5</v>
       </c>
@@ -5502,7 +5497,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10">
       <c r="A56" s="2" t="s">
         <v>5</v>
       </c>
@@ -5534,7 +5529,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10">
       <c r="A57" s="2" t="s">
         <v>5</v>
       </c>
@@ -5566,7 +5561,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10">
       <c r="A58" s="2" t="s">
         <v>5</v>
       </c>
@@ -5598,7 +5593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10">
       <c r="A59" s="2" t="s">
         <v>5</v>
       </c>
@@ -5630,7 +5625,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10">
       <c r="A60" s="2" t="s">
         <v>5</v>
       </c>
@@ -5662,7 +5657,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10">
       <c r="A61" s="2" t="s">
         <v>5</v>
       </c>
@@ -5694,7 +5689,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10">
       <c r="A62" s="2" t="s">
         <v>6</v>
       </c>
@@ -5726,7 +5721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10">
       <c r="A63" s="2" t="s">
         <v>6</v>
       </c>
@@ -5758,7 +5753,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10">
       <c r="A64" s="2" t="s">
         <v>6</v>
       </c>
@@ -5790,7 +5785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10">
       <c r="A65" s="2" t="s">
         <v>6</v>
       </c>
@@ -5822,7 +5817,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10">
       <c r="A66" s="2" t="s">
         <v>6</v>
       </c>
@@ -5854,7 +5849,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10">
       <c r="A67" s="2" t="s">
         <v>6</v>
       </c>
@@ -5886,7 +5881,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10">
       <c r="A68" s="2" t="s">
         <v>6</v>
       </c>
@@ -5918,7 +5913,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10">
       <c r="A69" s="2" t="s">
         <v>6</v>
       </c>
@@ -5950,7 +5945,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10">
       <c r="A70" s="2" t="s">
         <v>6</v>
       </c>
@@ -5982,7 +5977,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10">
       <c r="A71" s="2" t="s">
         <v>6</v>
       </c>
@@ -6014,7 +6009,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10">
       <c r="A72" s="2" t="s">
         <v>6</v>
       </c>
@@ -6046,7 +6041,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10">
       <c r="A73" s="2" t="s">
         <v>6</v>
       </c>
@@ -6078,7 +6073,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10">
       <c r="A74" s="2" t="s">
         <v>7</v>
       </c>
@@ -6110,7 +6105,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10">
       <c r="A75" s="2" t="s">
         <v>7</v>
       </c>
@@ -6142,7 +6137,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10">
       <c r="A76" s="2" t="s">
         <v>7</v>
       </c>
@@ -6174,7 +6169,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10">
       <c r="A77" s="2" t="s">
         <v>7</v>
       </c>
@@ -6206,7 +6201,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10">
       <c r="A78" s="2" t="s">
         <v>7</v>
       </c>
@@ -6238,7 +6233,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10">
       <c r="A79" s="2" t="s">
         <v>7</v>
       </c>
@@ -6270,7 +6265,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10">
       <c r="A80" s="2" t="s">
         <v>7</v>
       </c>
@@ -6302,7 +6297,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10">
       <c r="A81" s="2" t="s">
         <v>7</v>
       </c>
@@ -6334,7 +6329,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10">
       <c r="A82" s="2" t="s">
         <v>7</v>
       </c>
@@ -6366,7 +6361,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10">
       <c r="A83" s="2" t="s">
         <v>7</v>
       </c>
@@ -6398,7 +6393,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10">
       <c r="A84" s="2" t="s">
         <v>7</v>
       </c>
@@ -6430,7 +6425,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10">
       <c r="A85" s="2" t="s">
         <v>7</v>
       </c>
@@ -6462,7 +6457,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10">
       <c r="A86" s="2" t="s">
         <v>8</v>
       </c>
@@ -6494,7 +6489,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10">
       <c r="A87" s="2" t="s">
         <v>8</v>
       </c>
@@ -6526,7 +6521,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10">
       <c r="A88" s="2" t="s">
         <v>8</v>
       </c>
@@ -6558,7 +6553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10">
       <c r="A89" s="2" t="s">
         <v>8</v>
       </c>
@@ -6590,7 +6585,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10">
       <c r="A90" s="2" t="s">
         <v>8</v>
       </c>
@@ -6622,7 +6617,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10">
       <c r="A91" s="2" t="s">
         <v>8</v>
       </c>
@@ -6654,7 +6649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10">
       <c r="A92" s="2" t="s">
         <v>8</v>
       </c>
@@ -6686,7 +6681,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10">
       <c r="A93" s="2" t="s">
         <v>8</v>
       </c>
@@ -6718,7 +6713,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10">
       <c r="A94" s="2" t="s">
         <v>8</v>
       </c>
@@ -6750,7 +6745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10">
       <c r="A95" s="2" t="s">
         <v>8</v>
       </c>
@@ -6782,7 +6777,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10">
       <c r="A96" s="2" t="s">
         <v>8</v>
       </c>
@@ -6814,7 +6809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10">
       <c r="A97" s="2" t="s">
         <v>8</v>
       </c>
@@ -6846,7 +6841,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10">
       <c r="A98" s="2" t="s">
         <v>9</v>
       </c>
@@ -6878,7 +6873,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10">
       <c r="A99" s="2" t="s">
         <v>9</v>
       </c>
@@ -6910,7 +6905,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10">
       <c r="A100" s="2" t="s">
         <v>9</v>
       </c>
@@ -6942,7 +6937,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10">
       <c r="A101" s="2" t="s">
         <v>9</v>
       </c>
@@ -6974,7 +6969,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10">
       <c r="A102" s="2" t="s">
         <v>9</v>
       </c>
@@ -7006,7 +7001,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10">
       <c r="A103" s="2" t="s">
         <v>9</v>
       </c>
@@ -7038,7 +7033,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10">
       <c r="A104" s="2" t="s">
         <v>9</v>
       </c>
@@ -7070,7 +7065,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10">
       <c r="A105" s="2" t="s">
         <v>9</v>
       </c>
@@ -7102,7 +7097,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10">
       <c r="A106" s="2" t="s">
         <v>9</v>
       </c>
@@ -7134,7 +7129,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10">
       <c r="A107" s="2" t="s">
         <v>9</v>
       </c>
@@ -7166,7 +7161,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10">
       <c r="A108" s="2" t="s">
         <v>9</v>
       </c>
@@ -7198,7 +7193,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10">
       <c r="A109" s="2" t="s">
         <v>9</v>
       </c>
@@ -7230,7 +7225,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10">
       <c r="A110" s="2" t="s">
         <v>10</v>
       </c>
@@ -7262,7 +7257,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10">
       <c r="A111" s="2" t="s">
         <v>10</v>
       </c>
@@ -7294,7 +7289,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10">
       <c r="A112" s="2" t="s">
         <v>10</v>
       </c>
@@ -7326,7 +7321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10">
       <c r="A113" s="2" t="s">
         <v>10</v>
       </c>
@@ -7358,7 +7353,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10">
       <c r="A114" s="2" t="s">
         <v>10</v>
       </c>
@@ -7390,7 +7385,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10">
       <c r="A115" s="2" t="s">
         <v>10</v>
       </c>
@@ -7422,7 +7417,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10">
       <c r="A116" s="2" t="s">
         <v>10</v>
       </c>
@@ -7454,7 +7449,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10">
       <c r="A117" s="2" t="s">
         <v>10</v>
       </c>
@@ -7486,7 +7481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10">
       <c r="A118" s="2" t="s">
         <v>10</v>
       </c>
@@ -7518,7 +7513,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10">
       <c r="A119" s="2" t="s">
         <v>10</v>
       </c>
@@ -7550,7 +7545,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10">
       <c r="A120" s="2" t="s">
         <v>10</v>
       </c>
@@ -7582,7 +7577,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10">
       <c r="A121" s="2" t="s">
         <v>10</v>
       </c>
@@ -7614,7 +7609,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:10">
       <c r="A122" s="2" t="s">
         <v>11</v>
       </c>
@@ -7646,7 +7641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:10">
       <c r="A123" s="2" t="s">
         <v>11</v>
       </c>
@@ -7678,7 +7673,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:10">
       <c r="A124" s="2" t="s">
         <v>11</v>
       </c>
@@ -7710,7 +7705,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:10">
       <c r="A125" s="2" t="s">
         <v>11</v>
       </c>
@@ -7742,7 +7737,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:10">
       <c r="A126" s="2" t="s">
         <v>11</v>
       </c>
@@ -7774,7 +7769,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:10">
       <c r="A127" s="2" t="s">
         <v>11</v>
       </c>
@@ -7806,7 +7801,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:10">
       <c r="A128" s="2" t="s">
         <v>11</v>
       </c>
@@ -7838,7 +7833,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:10">
       <c r="A129" s="2" t="s">
         <v>11</v>
       </c>
@@ -7870,7 +7865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:10">
       <c r="A130" s="2" t="s">
         <v>11</v>
       </c>
@@ -7902,7 +7897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:10">
       <c r="A131" s="2" t="s">
         <v>11</v>
       </c>
@@ -7934,7 +7929,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:10">
       <c r="A132" s="2" t="s">
         <v>11</v>
       </c>
@@ -7966,7 +7961,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:10">
       <c r="A133" s="2" t="s">
         <v>11</v>
       </c>
@@ -7998,7 +7993,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:10">
       <c r="A134" s="2" t="s">
         <v>12</v>
       </c>
@@ -8030,7 +8025,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:10">
       <c r="A135" s="2" t="s">
         <v>12</v>
       </c>
@@ -8062,7 +8057,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:10">
       <c r="A136" s="2" t="s">
         <v>12</v>
       </c>
@@ -8094,7 +8089,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:10">
       <c r="A137" s="2" t="s">
         <v>12</v>
       </c>
@@ -8126,7 +8121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:10">
       <c r="A138" s="2" t="s">
         <v>12</v>
       </c>
@@ -8158,7 +8153,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:10">
       <c r="A139" s="2" t="s">
         <v>12</v>
       </c>
@@ -8190,7 +8185,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:10">
       <c r="A140" s="2" t="s">
         <v>12</v>
       </c>
@@ -8222,7 +8217,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:10">
       <c r="A141" s="2" t="s">
         <v>12</v>
       </c>
@@ -8254,7 +8249,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:10">
       <c r="A142" s="2" t="s">
         <v>12</v>
       </c>
@@ -8286,7 +8281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:10">
       <c r="A143" s="2" t="s">
         <v>12</v>
       </c>
@@ -8318,7 +8313,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:10">
       <c r="A144" s="2" t="s">
         <v>12</v>
       </c>
@@ -8350,7 +8345,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:10">
       <c r="A145" s="2" t="s">
         <v>12</v>
       </c>
@@ -8382,7 +8377,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:10">
       <c r="A146" s="2" t="s">
         <v>13</v>
       </c>
@@ -8414,7 +8409,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:10">
       <c r="A147" s="2" t="s">
         <v>13</v>
       </c>
@@ -8446,7 +8441,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:10">
       <c r="A148" s="2" t="s">
         <v>13</v>
       </c>
@@ -8478,7 +8473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:10">
       <c r="A149" s="2" t="s">
         <v>13</v>
       </c>
@@ -8510,7 +8505,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:10">
       <c r="A150" s="2" t="s">
         <v>13</v>
       </c>
@@ -8542,7 +8537,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:10">
       <c r="A151" s="2" t="s">
         <v>13</v>
       </c>
@@ -8574,7 +8569,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:10">
       <c r="A152" s="2" t="s">
         <v>13</v>
       </c>
@@ -8606,7 +8601,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:10">
       <c r="A153" s="2" t="s">
         <v>13</v>
       </c>
@@ -8638,7 +8633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:10">
       <c r="A154" s="2" t="s">
         <v>13</v>
       </c>
@@ -8670,7 +8665,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:10">
       <c r="A155" s="2" t="s">
         <v>13</v>
       </c>
@@ -8702,7 +8697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:10">
       <c r="A156" s="2" t="s">
         <v>13</v>
       </c>
@@ -8734,7 +8729,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:10">
       <c r="A157" s="2" t="s">
         <v>13</v>
       </c>
@@ -8766,7 +8761,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:10">
       <c r="A158" s="2" t="s">
         <v>14</v>
       </c>
@@ -8798,7 +8793,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:10">
       <c r="A159" s="2" t="s">
         <v>14</v>
       </c>
@@ -8830,7 +8825,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:10">
       <c r="A160" s="2" t="s">
         <v>14</v>
       </c>
@@ -8862,7 +8857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:10">
       <c r="A161" s="2" t="s">
         <v>14</v>
       </c>
@@ -8894,7 +8889,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:10">
       <c r="A162" s="2" t="s">
         <v>14</v>
       </c>
@@ -8926,7 +8921,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:10">
       <c r="A163" s="2" t="s">
         <v>14</v>
       </c>
@@ -8958,7 +8953,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:10">
       <c r="A164" s="2" t="s">
         <v>14</v>
       </c>
@@ -8990,7 +8985,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:10">
       <c r="A165" s="2" t="s">
         <v>14</v>
       </c>
@@ -9022,7 +9017,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:10">
       <c r="A166" s="2" t="s">
         <v>14</v>
       </c>
@@ -9054,7 +9049,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:10">
       <c r="A167" s="2" t="s">
         <v>14</v>
       </c>
@@ -9086,7 +9081,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:10">
       <c r="A168" s="2" t="s">
         <v>14</v>
       </c>
@@ -9118,7 +9113,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:10">
       <c r="A169" s="2" t="s">
         <v>14</v>
       </c>
@@ -9150,7 +9145,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:10">
       <c r="A170" s="2" t="s">
         <v>15</v>
       </c>
@@ -9182,7 +9177,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:10">
       <c r="A171" s="2" t="s">
         <v>15</v>
       </c>
@@ -9214,7 +9209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:10">
       <c r="A172" s="2" t="s">
         <v>15</v>
       </c>
@@ -9246,7 +9241,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:10">
       <c r="A173" s="2" t="s">
         <v>15</v>
       </c>
@@ -9278,7 +9273,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:10">
       <c r="A174" s="2" t="s">
         <v>15</v>
       </c>
@@ -9310,7 +9305,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:10">
       <c r="A175" s="2" t="s">
         <v>15</v>
       </c>
@@ -9342,7 +9337,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:10">
       <c r="A176" s="2" t="s">
         <v>15</v>
       </c>
@@ -9374,7 +9369,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:10">
       <c r="A177" s="2" t="s">
         <v>15</v>
       </c>
@@ -9406,7 +9401,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:10">
       <c r="A178" s="2" t="s">
         <v>15</v>
       </c>
@@ -9438,7 +9433,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:10">
       <c r="A179" s="2" t="s">
         <v>15</v>
       </c>
@@ -9470,7 +9465,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:10">
       <c r="A180" s="2" t="s">
         <v>15</v>
       </c>
@@ -9502,7 +9497,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:10">
       <c r="A181" s="2" t="s">
         <v>15</v>
       </c>
@@ -9534,7 +9529,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:10">
       <c r="A182" s="2" t="s">
         <v>16</v>
       </c>
@@ -9566,7 +9561,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:10">
       <c r="A183" s="2" t="s">
         <v>16</v>
       </c>
@@ -9598,7 +9593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:10">
       <c r="A184" s="2" t="s">
         <v>16</v>
       </c>
@@ -9630,7 +9625,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:10">
       <c r="A185" s="2" t="s">
         <v>16</v>
       </c>
@@ -9662,7 +9657,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:10">
       <c r="A186" s="2" t="s">
         <v>16</v>
       </c>
@@ -9694,7 +9689,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:10">
       <c r="A187" s="2" t="s">
         <v>16</v>
       </c>
@@ -9726,7 +9721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:10">
       <c r="A188" s="2" t="s">
         <v>16</v>
       </c>
@@ -9758,7 +9753,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:10">
       <c r="A189" s="2" t="s">
         <v>16</v>
       </c>
@@ -9790,7 +9785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:10">
       <c r="A190" s="2" t="s">
         <v>16</v>
       </c>
@@ -9822,7 +9817,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:10">
       <c r="A191" s="2" t="s">
         <v>16</v>
       </c>
@@ -9854,7 +9849,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:10">
       <c r="A192" s="2" t="s">
         <v>16</v>
       </c>
@@ -9886,7 +9881,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:10">
       <c r="A193" s="2" t="s">
         <v>16</v>
       </c>
@@ -9918,7 +9913,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:10">
       <c r="A194" s="2" t="s">
         <v>17</v>
       </c>
@@ -9940,8 +9935,8 @@
       <c r="G194" t="s">
         <v>57</v>
       </c>
-      <c r="H194">
-        <v>158.88</v>
+      <c r="H194" s="5">
+        <v>15888000</v>
       </c>
       <c r="I194">
         <v>0.29239999999999999</v>
@@ -9950,7 +9945,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:10">
       <c r="A195" s="2" t="s">
         <v>17</v>
       </c>
@@ -9982,7 +9977,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:10">
       <c r="A196" s="2" t="s">
         <v>17</v>
       </c>
@@ -10014,7 +10009,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:10">
       <c r="A197" s="2" t="s">
         <v>17</v>
       </c>
@@ -10046,7 +10041,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:10">
       <c r="A198" s="2" t="s">
         <v>17</v>
       </c>
@@ -10078,7 +10073,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:10">
       <c r="A199" s="2" t="s">
         <v>17</v>
       </c>
@@ -10110,7 +10105,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:10">
       <c r="A200" s="2" t="s">
         <v>17</v>
       </c>
@@ -10142,7 +10137,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:10">
       <c r="A201" s="2" t="s">
         <v>17</v>
       </c>
@@ -10174,7 +10169,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:10">
       <c r="A202" s="2" t="s">
         <v>17</v>
       </c>
@@ -10206,7 +10201,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:10">
       <c r="A203" s="2" t="s">
         <v>17</v>
       </c>
@@ -10238,7 +10233,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:10">
       <c r="A204" s="2" t="s">
         <v>17</v>
       </c>
@@ -10270,7 +10265,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:10">
       <c r="A205" s="2" t="s">
         <v>17</v>
       </c>
@@ -10302,7 +10297,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:10">
       <c r="A206" s="2" t="s">
         <v>18</v>
       </c>
@@ -10334,7 +10329,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:10">
       <c r="A207" s="2" t="s">
         <v>18</v>
       </c>
@@ -10366,7 +10361,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:10">
       <c r="A208" s="2" t="s">
         <v>18</v>
       </c>
@@ -10398,7 +10393,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:10">
       <c r="A209" s="2" t="s">
         <v>18</v>
       </c>
@@ -10430,7 +10425,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:10">
       <c r="A210" s="2" t="s">
         <v>18</v>
       </c>
@@ -10462,7 +10457,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:10">
       <c r="A211" s="2" t="s">
         <v>18</v>
       </c>
@@ -10494,7 +10489,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:10">
       <c r="A212" s="2" t="s">
         <v>18</v>
       </c>
@@ -10526,7 +10521,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:10">
       <c r="A213" s="2" t="s">
         <v>18</v>
       </c>
@@ -10558,7 +10553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:10">
       <c r="A214" s="2" t="s">
         <v>18</v>
       </c>
@@ -10590,7 +10585,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:10">
       <c r="A215" s="2" t="s">
         <v>18</v>
       </c>
@@ -10622,7 +10617,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:10">
       <c r="A216" s="2" t="s">
         <v>18</v>
       </c>
@@ -10654,7 +10649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:10">
       <c r="A217" s="2" t="s">
         <v>18</v>
       </c>
@@ -10686,7 +10681,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:10">
       <c r="A218" s="2" t="s">
         <v>19</v>
       </c>
@@ -10718,7 +10713,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:10">
       <c r="A219" s="2" t="s">
         <v>19</v>
       </c>
@@ -10750,7 +10745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:10">
       <c r="A220" s="2" t="s">
         <v>19</v>
       </c>
@@ -10782,7 +10777,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:10">
       <c r="A221" s="2" t="s">
         <v>19</v>
       </c>
@@ -10814,7 +10809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:10">
       <c r="A222" s="2" t="s">
         <v>19</v>
       </c>
@@ -10846,7 +10841,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="223" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:10">
       <c r="A223" s="2" t="s">
         <v>19</v>
       </c>
@@ -10878,7 +10873,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:10">
       <c r="A224" s="2" t="s">
         <v>19</v>
       </c>
@@ -10910,7 +10905,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:10">
       <c r="A225" s="2" t="s">
         <v>19</v>
       </c>
@@ -10942,7 +10937,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="226" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:10">
       <c r="A226" s="2" t="s">
         <v>19</v>
       </c>
@@ -10974,7 +10969,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="227" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:10">
       <c r="A227" s="2" t="s">
         <v>19</v>
       </c>
@@ -11006,7 +11001,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="228" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:10">
       <c r="A228" s="2" t="s">
         <v>19</v>
       </c>
@@ -11038,7 +11033,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="229" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:10">
       <c r="A229" s="2" t="s">
         <v>19</v>
       </c>
@@ -11070,7 +11065,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="230" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:10">
       <c r="A230" s="2" t="s">
         <v>20</v>
       </c>
@@ -11102,7 +11097,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="231" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:10">
       <c r="A231" s="2" t="s">
         <v>20</v>
       </c>
@@ -11134,7 +11129,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:10">
       <c r="A232" s="2" t="s">
         <v>20</v>
       </c>
@@ -11166,7 +11161,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:10">
       <c r="A233" s="2" t="s">
         <v>20</v>
       </c>
@@ -11198,7 +11193,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="234" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:10">
       <c r="A234" s="2" t="s">
         <v>20</v>
       </c>
@@ -11230,7 +11225,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="235" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:10">
       <c r="A235" s="2" t="s">
         <v>20</v>
       </c>
@@ -11262,7 +11257,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="236" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:10">
       <c r="A236" s="2" t="s">
         <v>20</v>
       </c>
@@ -11294,7 +11289,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="237" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:10">
       <c r="A237" s="2" t="s">
         <v>20</v>
       </c>
@@ -11326,7 +11321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="238" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:10">
       <c r="A238" s="2" t="s">
         <v>20</v>
       </c>
@@ -11358,7 +11353,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="239" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:10">
       <c r="A239" s="2" t="s">
         <v>20</v>
       </c>
@@ -11390,7 +11385,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="240" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:10">
       <c r="A240" s="2" t="s">
         <v>20</v>
       </c>
@@ -11422,7 +11417,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="241" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:10">
       <c r="A241" s="2" t="s">
         <v>20</v>
       </c>
@@ -11454,7 +11449,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="242" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:10">
       <c r="A242" s="2" t="s">
         <v>21</v>
       </c>
@@ -11486,7 +11481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="243" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:10">
       <c r="A243" s="2" t="s">
         <v>21</v>
       </c>
@@ -11518,7 +11513,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="244" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:10">
       <c r="A244" s="2" t="s">
         <v>21</v>
       </c>
@@ -11550,7 +11545,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="245" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:10">
       <c r="A245" s="2" t="s">
         <v>21</v>
       </c>
@@ -11582,7 +11577,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="246" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:10">
       <c r="A246" s="2" t="s">
         <v>21</v>
       </c>
@@ -11614,7 +11609,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="247" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:10">
       <c r="A247" s="2" t="s">
         <v>21</v>
       </c>
@@ -11646,7 +11641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="248" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:10">
       <c r="A248" s="2" t="s">
         <v>21</v>
       </c>
@@ -11678,7 +11673,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="249" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:10">
       <c r="A249" s="2" t="s">
         <v>21</v>
       </c>
@@ -11710,7 +11705,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="250" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:10">
       <c r="A250" s="2" t="s">
         <v>21</v>
       </c>
@@ -11742,7 +11737,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="251" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:10">
       <c r="A251" s="2" t="s">
         <v>21</v>
       </c>
@@ -11774,7 +11769,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="252" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:10">
       <c r="A252" s="2" t="s">
         <v>21</v>
       </c>
@@ -11806,7 +11801,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="253" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:10">
       <c r="A253" s="2" t="s">
         <v>21</v>
       </c>
@@ -11838,7 +11833,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="254" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:10">
       <c r="A254" s="2" t="s">
         <v>22</v>
       </c>
@@ -11870,7 +11865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="255" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:10">
       <c r="A255" s="2" t="s">
         <v>22</v>
       </c>
@@ -11902,7 +11897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="256" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:10">
       <c r="A256" s="2" t="s">
         <v>22</v>
       </c>
@@ -11934,7 +11929,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="257" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:10">
       <c r="A257" s="2" t="s">
         <v>22</v>
       </c>
@@ -11966,7 +11961,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="258" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:10">
       <c r="A258" s="2" t="s">
         <v>22</v>
       </c>
@@ -11998,7 +11993,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="259" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:10">
       <c r="A259" s="2" t="s">
         <v>22</v>
       </c>
@@ -12030,7 +12025,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="260" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:10">
       <c r="A260" s="2" t="s">
         <v>22</v>
       </c>
@@ -12062,7 +12057,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="261" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:10">
       <c r="A261" s="2" t="s">
         <v>22</v>
       </c>
@@ -12094,7 +12089,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="262" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:10">
       <c r="A262" s="2" t="s">
         <v>22</v>
       </c>
@@ -12126,7 +12121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="263" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:10">
       <c r="A263" s="2" t="s">
         <v>22</v>
       </c>
@@ -12158,7 +12153,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="264" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:10">
       <c r="A264" s="2" t="s">
         <v>22</v>
       </c>
@@ -12190,7 +12185,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="265" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:10">
       <c r="A265" s="2" t="s">
         <v>22</v>
       </c>
@@ -12222,7 +12217,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="266" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:10">
       <c r="A266" s="2" t="s">
         <v>23</v>
       </c>
@@ -12254,7 +12249,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="267" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:10">
       <c r="A267" s="2" t="s">
         <v>23</v>
       </c>
@@ -12286,7 +12281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="268" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:10">
       <c r="A268" s="2" t="s">
         <v>23</v>
       </c>
@@ -12318,7 +12313,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="269" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:10">
       <c r="A269" s="2" t="s">
         <v>23</v>
       </c>
@@ -12350,7 +12345,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="270" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:10">
       <c r="A270" s="2" t="s">
         <v>23</v>
       </c>
@@ -12382,7 +12377,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="271" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:10">
       <c r="A271" s="2" t="s">
         <v>23</v>
       </c>
@@ -12414,7 +12409,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="272" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:10">
       <c r="A272" s="2" t="s">
         <v>23</v>
       </c>
@@ -12446,7 +12441,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="273" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:10">
       <c r="A273" s="2" t="s">
         <v>23</v>
       </c>
@@ -12478,7 +12473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="274" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:10">
       <c r="A274" s="2" t="s">
         <v>23</v>
       </c>
@@ -12510,7 +12505,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="275" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:10">
       <c r="A275" s="2" t="s">
         <v>23</v>
       </c>
@@ -12542,7 +12537,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="276" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:10">
       <c r="A276" s="2" t="s">
         <v>23</v>
       </c>
@@ -12574,7 +12569,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="277" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:10">
       <c r="A277" s="2" t="s">
         <v>23</v>
       </c>
@@ -12606,7 +12601,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="278" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:10">
       <c r="A278" s="2" t="s">
         <v>24</v>
       </c>
@@ -12638,7 +12633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="279" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:10">
       <c r="A279" s="2" t="s">
         <v>24</v>
       </c>
@@ -12670,7 +12665,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="280" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:10">
       <c r="A280" s="2" t="s">
         <v>24</v>
       </c>
@@ -12702,7 +12697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="281" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:10">
       <c r="A281" s="2" t="s">
         <v>24</v>
       </c>
@@ -12734,7 +12729,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="282" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:10">
       <c r="A282" s="2" t="s">
         <v>24</v>
       </c>
@@ -12766,7 +12761,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="283" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:10">
       <c r="A283" s="2" t="s">
         <v>24</v>
       </c>
@@ -12798,7 +12793,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="284" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:10">
       <c r="A284" s="2" t="s">
         <v>24</v>
       </c>
@@ -12830,7 +12825,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="285" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:10">
       <c r="A285" s="2" t="s">
         <v>24</v>
       </c>
@@ -12862,7 +12857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="286" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:10">
       <c r="A286" s="2" t="s">
         <v>24</v>
       </c>
@@ -12894,7 +12889,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="287" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:10">
       <c r="A287" s="2" t="s">
         <v>24</v>
       </c>
@@ -12926,7 +12921,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="288" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:10">
       <c r="A288" s="2" t="s">
         <v>24</v>
       </c>
@@ -12958,7 +12953,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="289" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:10">
       <c r="A289" s="2" t="s">
         <v>24</v>
       </c>
@@ -12990,7 +12985,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="290" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:10">
       <c r="A290" s="2" t="s">
         <v>25</v>
       </c>
@@ -13022,7 +13017,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="291" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:10">
       <c r="A291" s="2" t="s">
         <v>25</v>
       </c>
@@ -13054,7 +13049,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="292" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:10">
       <c r="A292" s="2" t="s">
         <v>25</v>
       </c>
@@ -13086,7 +13081,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="293" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:10">
       <c r="A293" s="2" t="s">
         <v>25</v>
       </c>
@@ -13118,7 +13113,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="294" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:10">
       <c r="A294" s="2" t="s">
         <v>25</v>
       </c>
@@ -13150,7 +13145,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="295" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:10">
       <c r="A295" s="2" t="s">
         <v>25</v>
       </c>
@@ -13182,7 +13177,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="296" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:10">
       <c r="A296" s="2" t="s">
         <v>25</v>
       </c>
@@ -13214,7 +13209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="297" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:10">
       <c r="A297" s="2" t="s">
         <v>25</v>
       </c>
@@ -13246,7 +13241,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="298" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:10">
       <c r="A298" s="2" t="s">
         <v>25</v>
       </c>
@@ -13278,7 +13273,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="299" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:10">
       <c r="A299" s="2" t="s">
         <v>25</v>
       </c>
@@ -13310,7 +13305,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="300" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:10">
       <c r="A300" s="2" t="s">
         <v>25</v>
       </c>
@@ -13342,7 +13337,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="301" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:10">
       <c r="A301" s="2" t="s">
         <v>25</v>
       </c>
@@ -13374,7 +13369,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="302" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:10">
       <c r="A302" s="2" t="s">
         <v>26</v>
       </c>
@@ -13406,7 +13401,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="303" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:10">
       <c r="A303" s="2" t="s">
         <v>26</v>
       </c>
@@ -13438,7 +13433,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="304" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:10">
       <c r="A304" s="2" t="s">
         <v>26</v>
       </c>
@@ -13470,7 +13465,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="305" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:10">
       <c r="A305" s="2" t="s">
         <v>26</v>
       </c>
@@ -13502,7 +13497,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="306" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:10">
       <c r="A306" s="2" t="s">
         <v>26</v>
       </c>
@@ -13534,7 +13529,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="307" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:10">
       <c r="A307" s="2" t="s">
         <v>26</v>
       </c>
@@ -13566,7 +13561,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="308" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:10">
       <c r="A308" s="2" t="s">
         <v>26</v>
       </c>
@@ -13598,7 +13593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="309" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:10">
       <c r="A309" s="2" t="s">
         <v>26</v>
       </c>
@@ -13630,7 +13625,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="310" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:10">
       <c r="A310" s="2" t="s">
         <v>26</v>
       </c>
@@ -13662,7 +13657,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="311" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:10">
       <c r="A311" s="2" t="s">
         <v>26</v>
       </c>
@@ -13694,7 +13689,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="312" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:10">
       <c r="A312" s="2" t="s">
         <v>26</v>
       </c>
@@ -13726,7 +13721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="313" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:10">
       <c r="A313" s="2" t="s">
         <v>26</v>
       </c>
@@ -13758,7 +13753,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="314" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:10">
       <c r="A314" s="2" t="s">
         <v>27</v>
       </c>
@@ -13790,7 +13785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="315" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:10">
       <c r="A315" s="2" t="s">
         <v>27</v>
       </c>
@@ -13822,7 +13817,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="316" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:10">
       <c r="A316" s="2" t="s">
         <v>27</v>
       </c>
@@ -13854,7 +13849,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="317" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:10">
       <c r="A317" s="2" t="s">
         <v>27</v>
       </c>
@@ -13886,7 +13881,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="318" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:10">
       <c r="A318" s="2" t="s">
         <v>27</v>
       </c>
@@ -13918,7 +13913,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="319" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:10">
       <c r="A319" s="2" t="s">
         <v>27</v>
       </c>
@@ -13950,7 +13945,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="320" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:10">
       <c r="A320" s="2" t="s">
         <v>27</v>
       </c>
@@ -13982,7 +13977,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="321" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:10">
       <c r="A321" s="2" t="s">
         <v>27</v>
       </c>
@@ -14014,7 +14009,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="322" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:10">
       <c r="A322" s="2" t="s">
         <v>27</v>
       </c>
@@ -14046,7 +14041,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="323" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:10">
       <c r="A323" s="2" t="s">
         <v>27</v>
       </c>
@@ -14078,7 +14073,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="324" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:10">
       <c r="A324" s="2" t="s">
         <v>27</v>
       </c>
@@ -14110,7 +14105,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="325" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:10">
       <c r="A325" s="2" t="s">
         <v>27</v>
       </c>
@@ -14142,7 +14137,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="326" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:10">
       <c r="A326" s="2" t="s">
         <v>28</v>
       </c>
@@ -14174,7 +14169,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="327" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:10">
       <c r="A327" s="2" t="s">
         <v>28</v>
       </c>
@@ -14206,7 +14201,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="328" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:10">
       <c r="A328" s="2" t="s">
         <v>28</v>
       </c>
@@ -14238,7 +14233,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="329" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:10">
       <c r="A329" s="2" t="s">
         <v>28</v>
       </c>
@@ -14270,7 +14265,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="330" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:10">
       <c r="A330" s="2" t="s">
         <v>28</v>
       </c>
@@ -14302,7 +14297,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="331" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:10">
       <c r="A331" s="2" t="s">
         <v>28</v>
       </c>
@@ -14334,7 +14329,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="332" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:10">
       <c r="A332" s="2" t="s">
         <v>28</v>
       </c>
@@ -14366,7 +14361,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="333" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:10">
       <c r="A333" s="2" t="s">
         <v>28</v>
       </c>
@@ -14398,7 +14393,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="334" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:10">
       <c r="A334" s="2" t="s">
         <v>28</v>
       </c>
@@ -14430,7 +14425,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="335" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:10">
       <c r="A335" s="2" t="s">
         <v>28</v>
       </c>
@@ -14462,7 +14457,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="336" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:10">
       <c r="A336" s="2" t="s">
         <v>28</v>
       </c>
@@ -14494,7 +14489,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="337" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:10">
       <c r="A337" s="2" t="s">
         <v>28</v>
       </c>
@@ -14526,7 +14521,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="338" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:10">
       <c r="A338" s="2" t="s">
         <v>29</v>
       </c>
@@ -14558,7 +14553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="339" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:10">
       <c r="A339" s="2" t="s">
         <v>29</v>
       </c>
@@ -14590,7 +14585,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="340" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:10">
       <c r="A340" s="2" t="s">
         <v>29</v>
       </c>
@@ -14622,7 +14617,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="341" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:10">
       <c r="A341" s="2" t="s">
         <v>29</v>
       </c>
@@ -14654,7 +14649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="342" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:10">
       <c r="A342" s="2" t="s">
         <v>29</v>
       </c>
@@ -14686,7 +14681,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="343" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:10">
       <c r="A343" s="2" t="s">
         <v>29</v>
       </c>
@@ -14718,7 +14713,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="344" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:10">
       <c r="A344" s="2" t="s">
         <v>29</v>
       </c>
@@ -14750,7 +14745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="345" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:10">
       <c r="A345" s="2" t="s">
         <v>29</v>
       </c>
@@ -14782,7 +14777,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="346" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:10">
       <c r="A346" s="2" t="s">
         <v>29</v>
       </c>
@@ -14814,7 +14809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="347" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:10">
       <c r="A347" s="2" t="s">
         <v>29</v>
       </c>
@@ -14846,7 +14841,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="348" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:10">
       <c r="A348" s="2" t="s">
         <v>29</v>
       </c>
@@ -14878,7 +14873,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="349" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:10">
       <c r="A349" s="2" t="s">
         <v>29</v>
       </c>
@@ -14910,7 +14905,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="350" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:10">
       <c r="A350" s="2" t="s">
         <v>30</v>
       </c>
@@ -14942,7 +14937,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="351" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:10">
       <c r="A351" s="2" t="s">
         <v>30</v>
       </c>
@@ -14974,7 +14969,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="352" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:10">
       <c r="A352" s="2" t="s">
         <v>30</v>
       </c>
@@ -15006,7 +15001,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="353" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:10">
       <c r="A353" s="2" t="s">
         <v>30</v>
       </c>
@@ -15038,7 +15033,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="354" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:10">
       <c r="A354" s="2" t="s">
         <v>30</v>
       </c>
@@ -15070,7 +15065,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="355" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:10">
       <c r="A355" s="2" t="s">
         <v>30</v>
       </c>
@@ -15102,7 +15097,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="356" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:10">
       <c r="A356" s="2" t="s">
         <v>30</v>
       </c>
@@ -15134,7 +15129,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="357" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:10">
       <c r="A357" s="2" t="s">
         <v>30</v>
       </c>
@@ -15166,7 +15161,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="358" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:10">
       <c r="A358" s="2" t="s">
         <v>30</v>
       </c>
@@ -15198,7 +15193,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="359" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:10">
       <c r="A359" s="2" t="s">
         <v>30</v>
       </c>
@@ -15230,7 +15225,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="360" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:10">
       <c r="A360" s="2" t="s">
         <v>30</v>
       </c>
@@ -15262,7 +15257,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="361" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:10">
       <c r="A361" s="2" t="s">
         <v>30</v>
       </c>
@@ -15294,7 +15289,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="362" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:10">
       <c r="A362" s="2" t="s">
         <v>31</v>
       </c>
@@ -15326,7 +15321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="363" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:10">
       <c r="A363" s="2" t="s">
         <v>31</v>
       </c>
@@ -15358,7 +15353,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="364" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:10">
       <c r="A364" s="2" t="s">
         <v>31</v>
       </c>
@@ -15390,7 +15385,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="365" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:10">
       <c r="A365" s="2" t="s">
         <v>31</v>
       </c>
@@ -15422,7 +15417,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="366" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:10">
       <c r="A366" s="2" t="s">
         <v>31</v>
       </c>
@@ -15454,7 +15449,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="367" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:10">
       <c r="A367" s="2" t="s">
         <v>31</v>
       </c>
@@ -15486,7 +15481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="368" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:10">
       <c r="A368" s="2" t="s">
         <v>31</v>
       </c>
@@ -15518,7 +15513,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="369" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:10">
       <c r="A369" s="2" t="s">
         <v>31</v>
       </c>
@@ -15550,7 +15545,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="370" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:10">
       <c r="A370" s="2" t="s">
         <v>31</v>
       </c>
@@ -15582,7 +15577,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="371" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:10">
       <c r="A371" s="2" t="s">
         <v>31</v>
       </c>
@@ -15614,7 +15609,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="372" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:10">
       <c r="A372" s="2" t="s">
         <v>31</v>
       </c>
@@ -15646,7 +15641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="373" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:10">
       <c r="A373" s="2" t="s">
         <v>31</v>
       </c>
@@ -15678,7 +15673,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="374" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:10">
       <c r="A374" s="2" t="s">
         <v>32</v>
       </c>
@@ -15710,7 +15705,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="375" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:10">
       <c r="A375" s="2" t="s">
         <v>32</v>
       </c>
@@ -15742,7 +15737,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="376" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:10">
       <c r="A376" s="2" t="s">
         <v>32</v>
       </c>
@@ -15774,7 +15769,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="377" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:10">
       <c r="A377" s="2" t="s">
         <v>32</v>
       </c>
@@ -15806,7 +15801,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="378" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:10">
       <c r="A378" s="2" t="s">
         <v>32</v>
       </c>
@@ -15838,7 +15833,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="379" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:10">
       <c r="A379" s="2" t="s">
         <v>32</v>
       </c>
@@ -15870,7 +15865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="380" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:10">
       <c r="A380" s="2" t="s">
         <v>32</v>
       </c>
@@ -15902,7 +15897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="381" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:10">
       <c r="A381" s="2" t="s">
         <v>32</v>
       </c>
@@ -15934,7 +15929,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="382" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:10">
       <c r="A382" s="2" t="s">
         <v>32</v>
       </c>
@@ -15966,7 +15961,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="383" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:10">
       <c r="A383" s="2" t="s">
         <v>32</v>
       </c>
@@ -15998,7 +15993,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="384" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:10">
       <c r="A384" s="2" t="s">
         <v>32</v>
       </c>
@@ -16030,7 +16025,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="385" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:10">
       <c r="A385" s="2" t="s">
         <v>32</v>
       </c>
@@ -16062,7 +16057,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="386" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:10">
       <c r="A386" s="2" t="s">
         <v>33</v>
       </c>
@@ -16094,7 +16089,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="387" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:10">
       <c r="A387" s="2" t="s">
         <v>33</v>
       </c>
@@ -16126,7 +16121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="388" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:10">
       <c r="A388" s="2" t="s">
         <v>33</v>
       </c>
@@ -16158,7 +16153,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="389" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:10">
       <c r="A389" s="2" t="s">
         <v>33</v>
       </c>
@@ -16190,7 +16185,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="390" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:10">
       <c r="A390" s="2" t="s">
         <v>33</v>
       </c>
@@ -16222,7 +16217,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="391" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:10">
       <c r="A391" s="2" t="s">
         <v>33</v>
       </c>
@@ -16254,7 +16249,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="392" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:10">
       <c r="A392" s="2" t="s">
         <v>33</v>
       </c>
@@ -16286,7 +16281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="393" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:10">
       <c r="A393" s="2" t="s">
         <v>33</v>
       </c>
@@ -16318,7 +16313,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="394" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:10">
       <c r="A394" s="2" t="s">
         <v>33</v>
       </c>
@@ -16350,7 +16345,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="395" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:10">
       <c r="A395" s="2" t="s">
         <v>33</v>
       </c>
@@ -16382,7 +16377,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="396" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:10">
       <c r="A396" s="2" t="s">
         <v>33</v>
       </c>
@@ -16414,7 +16409,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="397" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:10">
       <c r="A397" s="2" t="s">
         <v>33</v>
       </c>
@@ -16446,7 +16441,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="398" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:10">
       <c r="A398" s="2" t="s">
         <v>34</v>
       </c>
@@ -16478,7 +16473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="399" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:10">
       <c r="A399" s="2" t="s">
         <v>34</v>
       </c>
@@ -16510,7 +16505,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="400" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:10">
       <c r="A400" s="2" t="s">
         <v>34</v>
       </c>
@@ -16542,7 +16537,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="401" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:10">
       <c r="A401" s="2" t="s">
         <v>34</v>
       </c>
@@ -16574,7 +16569,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="402" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:10">
       <c r="A402" s="2" t="s">
         <v>34</v>
       </c>
@@ -16606,7 +16601,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="403" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:10">
       <c r="A403" s="2" t="s">
         <v>34</v>
       </c>
@@ -16638,7 +16633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="404" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:10">
       <c r="A404" s="2" t="s">
         <v>34</v>
       </c>
@@ -16670,7 +16665,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="405" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:10">
       <c r="A405" s="2" t="s">
         <v>34</v>
       </c>
@@ -16702,7 +16697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="406" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:10">
       <c r="A406" s="2" t="s">
         <v>34</v>
       </c>
@@ -16734,7 +16729,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="407" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:10">
       <c r="A407" s="2" t="s">
         <v>34</v>
       </c>
@@ -16766,7 +16761,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="408" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:10">
       <c r="A408" s="2" t="s">
         <v>34</v>
       </c>
@@ -16798,7 +16793,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="409" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:10">
       <c r="A409" s="2" t="s">
         <v>34</v>
       </c>
@@ -16830,7 +16825,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="410" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:10">
       <c r="A410" s="2" t="s">
         <v>35</v>
       </c>
@@ -16862,7 +16857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="411" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:10">
       <c r="A411" s="2" t="s">
         <v>35</v>
       </c>
@@ -16894,7 +16889,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="412" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:10">
       <c r="A412" s="2" t="s">
         <v>35</v>
       </c>
@@ -16926,7 +16921,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="413" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:10">
       <c r="A413" s="2" t="s">
         <v>35</v>
       </c>
@@ -16958,7 +16953,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="414" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:10">
       <c r="A414" s="2" t="s">
         <v>35</v>
       </c>
@@ -16990,7 +16985,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="415" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:10">
       <c r="A415" s="2" t="s">
         <v>35</v>
       </c>
@@ -17022,7 +17017,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="416" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:10">
       <c r="A416" s="2" t="s">
         <v>35</v>
       </c>
@@ -17054,7 +17049,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="417" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:10">
       <c r="A417" s="2" t="s">
         <v>35</v>
       </c>
@@ -17086,7 +17081,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="418" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:10">
       <c r="A418" s="2" t="s">
         <v>35</v>
       </c>
@@ -17118,7 +17113,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="419" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:10">
       <c r="A419" s="2" t="s">
         <v>35</v>
       </c>
@@ -17150,7 +17145,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="420" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:10">
       <c r="A420" s="2" t="s">
         <v>35</v>
       </c>
@@ -17182,7 +17177,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="421" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:10">
       <c r="A421" s="2" t="s">
         <v>35</v>
       </c>
@@ -17214,7 +17209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="422" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:10">
       <c r="A422" s="2" t="s">
         <v>36</v>
       </c>
@@ -17246,7 +17241,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="423" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:10">
       <c r="A423" s="2" t="s">
         <v>36</v>
       </c>
@@ -17278,7 +17273,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="424" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:10">
       <c r="A424" s="2" t="s">
         <v>36</v>
       </c>
@@ -17310,7 +17305,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="425" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:10">
       <c r="A425" s="2" t="s">
         <v>36</v>
       </c>
@@ -17342,7 +17337,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="426" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:10">
       <c r="A426" s="2" t="s">
         <v>36</v>
       </c>
@@ -17374,7 +17369,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="427" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:10">
       <c r="A427" s="2" t="s">
         <v>36</v>
       </c>
@@ -17406,7 +17401,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="428" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:10">
       <c r="A428" s="2" t="s">
         <v>36</v>
       </c>
@@ -17438,7 +17433,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="429" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:10">
       <c r="A429" s="2" t="s">
         <v>36</v>
       </c>
@@ -17470,7 +17465,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="430" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:10">
       <c r="A430" s="2" t="s">
         <v>36</v>
       </c>
@@ -17502,7 +17497,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="431" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:10">
       <c r="A431" s="2" t="s">
         <v>36</v>
       </c>
@@ -17534,7 +17529,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="432" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:10">
       <c r="A432" s="2" t="s">
         <v>36</v>
       </c>
@@ -17566,7 +17561,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="433" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:25">
       <c r="A433" s="2" t="s">
         <v>36</v>
       </c>
@@ -17598,7 +17593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="434" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:25">
       <c r="A434" s="2" t="s">
         <v>37</v>
       </c>
@@ -17639,7 +17634,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="435" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:25">
       <c r="A435" s="2" t="s">
         <v>37</v>
       </c>
@@ -17677,7 +17672,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="436" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:25">
       <c r="A436" s="2" t="s">
         <v>37</v>
       </c>
@@ -17715,7 +17710,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="437" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:25">
       <c r="A437" s="2" t="s">
         <v>37</v>
       </c>
@@ -17753,7 +17748,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="438" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:25">
       <c r="A438" s="2" t="s">
         <v>37</v>
       </c>
@@ -17791,7 +17786,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="439" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:25">
       <c r="A439" s="2" t="s">
         <v>37</v>
       </c>
@@ -17829,7 +17824,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="440" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:25">
       <c r="A440" s="2" t="s">
         <v>37</v>
       </c>
@@ -17867,7 +17862,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="441" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:25">
       <c r="A441" s="2" t="s">
         <v>37</v>
       </c>
@@ -17905,7 +17900,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="442" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:25">
       <c r="A442" s="2" t="s">
         <v>37</v>
       </c>
@@ -17943,7 +17938,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="443" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:25">
       <c r="A443" s="2" t="s">
         <v>37</v>
       </c>
@@ -17981,7 +17976,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="444" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:25">
       <c r="A444" s="2" t="s">
         <v>37</v>
       </c>
@@ -18019,7 +18014,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="445" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:25">
       <c r="A445" s="2" t="s">
         <v>37</v>
       </c>
@@ -18057,7 +18052,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="446" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:25">
       <c r="A446" s="2" t="s">
         <v>38</v>
       </c>
@@ -18095,7 +18090,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="447" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:25">
       <c r="A447" s="2" t="s">
         <v>38</v>
       </c>
@@ -18133,7 +18128,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="448" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:25">
       <c r="A448" s="2" t="s">
         <v>38</v>
       </c>
@@ -18171,7 +18166,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="449" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:25">
       <c r="A449" s="2" t="s">
         <v>38</v>
       </c>
@@ -18209,7 +18204,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="450" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:25">
       <c r="A450" s="2" t="s">
         <v>38</v>
       </c>
@@ -18247,7 +18242,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="451" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:25">
       <c r="A451" s="2" t="s">
         <v>38</v>
       </c>
@@ -18285,7 +18280,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="452" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:25">
       <c r="A452" s="2" t="s">
         <v>38</v>
       </c>
@@ -18323,7 +18318,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="453" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:25">
       <c r="A453" s="2" t="s">
         <v>38</v>
       </c>
@@ -18361,7 +18356,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="454" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:25">
       <c r="A454" s="2" t="s">
         <v>38</v>
       </c>
@@ -18399,7 +18394,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="455" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:25">
       <c r="A455" s="2" t="s">
         <v>38</v>
       </c>
@@ -18437,7 +18432,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="456" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:25">
       <c r="A456" s="2" t="s">
         <v>38</v>
       </c>
@@ -18475,7 +18470,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="457" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:25">
       <c r="A457" s="2" t="s">
         <v>38</v>
       </c>
@@ -18513,7 +18508,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="458" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:25">
       <c r="A458" s="2" t="s">
         <v>39</v>
       </c>
@@ -18551,7 +18546,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="459" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:25">
       <c r="A459" s="2" t="s">
         <v>39</v>
       </c>
@@ -18589,7 +18584,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="460" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:25">
       <c r="A460" s="2" t="s">
         <v>39</v>
       </c>
@@ -18627,7 +18622,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="461" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:25">
       <c r="A461" s="2" t="s">
         <v>39</v>
       </c>
@@ -18665,7 +18660,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="462" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:25">
       <c r="A462" s="2" t="s">
         <v>39</v>
       </c>
@@ -18703,7 +18698,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="463" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:25">
       <c r="A463" s="2" t="s">
         <v>39</v>
       </c>
@@ -18741,7 +18736,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="464" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:25">
       <c r="A464" s="2" t="s">
         <v>39</v>
       </c>
@@ -18779,7 +18774,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="465" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:25">
       <c r="A465" s="2" t="s">
         <v>39</v>
       </c>
@@ -18817,7 +18812,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="466" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:25">
       <c r="A466" s="2" t="s">
         <v>39</v>
       </c>
@@ -18855,7 +18850,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="467" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:25">
       <c r="A467" s="2" t="s">
         <v>39</v>
       </c>
@@ -18893,7 +18888,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="468" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:25">
       <c r="A468" s="2" t="s">
         <v>39</v>
       </c>
@@ -18931,7 +18926,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="469" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:25">
       <c r="A469" s="2" t="s">
         <v>39</v>
       </c>
@@ -18970,7 +18965,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Z469" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <autoFilter ref="A1:Z469"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>

<commit_message>
intento de optimización. Tarda demasiado. + otros cambios
</commit_message>
<xml_diff>
--- a/InputCMPC.xlsx
+++ b/InputCMPC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ite02\Documents\Gaston\CMPC-manufacturing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2889E22-EE9B-48AD-8ED7-73612226CA5B}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B636B725-F8B9-4CA6-8A54-75C68AD67C21}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16695" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1219,8 +1219,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M469"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" topLeftCell="A445" workbookViewId="0">
+      <selection activeCell="C460" sqref="C460"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>

</xml_diff>

<commit_message>
Muchos cambios que ligaban a chile todavía en las lineas de produccion. Fijarse que da backorders en la linea 3. Si los datos tienen sentido
</commit_message>
<xml_diff>
--- a/InputCMPC.xlsx
+++ b/InputCMPC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ite02\Documents\Gaston\CMPC-manufacturing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B636B725-F8B9-4CA6-8A54-75C68AD67C21}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FFF3FB3-DA33-4601-8D15-09E7D3111E4A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16695" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1219,8 +1219,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M469"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A445" workbookViewId="0">
-      <selection activeCell="C460" sqref="C460"/>
+    <sheetView tabSelected="1" topLeftCell="A183" workbookViewId="0">
+      <selection activeCell="H194" sqref="H194"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -9171,7 +9171,7 @@
         <v>3</v>
       </c>
       <c r="H194" s="4">
-        <v>15888000</v>
+        <v>15888</v>
       </c>
       <c r="I194">
         <v>0.29239999999999999</v>

</xml_diff>

<commit_message>
incorporacion de parametros de calculo
</commit_message>
<xml_diff>
--- a/InputCMPC.xlsx
+++ b/InputCMPC.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24426"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ite02\Documents\Gaston\Source\CMPC-manufacturing\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D740E99C-B72E-4A72-8313-E4ED800C63A6}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16695" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16700" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="SKU" sheetId="4" r:id="rId1"/>
     <sheet name="Lead Times" sheetId="5" r:id="rId2"/>
+    <sheet name="Lines" sheetId="6" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">SKU!$A$1:$M$469</definedName>
@@ -29,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1908" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1920" uniqueCount="97">
   <si>
     <t>100-AAA-05-016</t>
   </si>
@@ -288,21 +283,53 @@
   <si>
     <t>packets_per_pallet</t>
   </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>mano_obraD_cant_turno</t>
+  </si>
+  <si>
+    <t>mano_obraD_costo_turno</t>
+  </si>
+  <si>
+    <t>mano_obraI_cant_turno</t>
+  </si>
+  <si>
+    <t>mano_obraI_costo_turno</t>
+  </si>
+  <si>
+    <t>mano_obra_CO_hora</t>
+  </si>
+  <si>
+    <t>mantenimiento_turno</t>
+  </si>
+  <si>
+    <t>gastos_generales_mes</t>
+  </si>
+  <si>
+    <t>costosCO_CO</t>
+  </si>
+  <si>
+    <t>merma</t>
+  </si>
+  <si>
+    <t>line_type</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -656,15 +683,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="283" applyFont="1"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="283" applyFont="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="283" applyFont="1"/>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" xfId="283" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="284">
@@ -1287,29 +1314,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S469"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="14.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.875" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.83203125" style="4" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.75" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="19" width="6.625" bestFit="1" customWidth="1"/>
+    <col min="14" max="19" width="6.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
@@ -28984,7 +29011,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M469" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <autoFilter ref="A1:M469"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
@@ -28996,14 +29023,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1498B488-EC29-409A-A4D1-C2D6F69144FE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
@@ -29268,5 +29295,80 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="2" width="14.1640625" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" customWidth="1"/>
+    <col min="4" max="4" width="22.1640625" customWidth="1"/>
+    <col min="5" max="5" width="23.33203125" customWidth="1"/>
+    <col min="6" max="6" width="21.83203125" customWidth="1"/>
+    <col min="7" max="7" width="23.1640625" customWidth="1"/>
+    <col min="8" max="8" width="22.1640625" customWidth="1"/>
+    <col min="9" max="9" width="21.33203125" customWidth="1"/>
+    <col min="10" max="10" width="21.6640625" customWidth="1"/>
+    <col min="11" max="11" width="21.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I1" t="s">
+        <v>92</v>
+      </c>
+      <c r="J1" t="s">
+        <v>93</v>
+      </c>
+      <c r="K1" t="s">
+        <v>94</v>
+      </c>
+      <c r="L1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>